<commit_message>
allow script to be re-run multiple times, and fix a minor bug with prepending 'properties.' on re-runs
</commit_message>
<xml_diff>
--- a/sync_commcare_assets/contact-source-target-mappings.xlsx
+++ b/sync_commcare_assets/contact-source-target-mappings.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="513">
   <si>
     <t>Data Source</t>
   </si>
@@ -53,1513 +53,1507 @@
     <t>case_id</t>
   </si>
   <si>
-    <t>properties.properties.caseid</t>
-  </si>
-  <si>
     <t>able_to_test</t>
   </si>
   <si>
-    <t>properties.properties.properties.able_to_test</t>
+    <t>properties.able_to_test</t>
   </si>
   <si>
     <t>address</t>
   </si>
   <si>
-    <t>properties.properties.properties.address</t>
+    <t>properties.address</t>
   </si>
   <si>
     <t>address_city</t>
   </si>
   <si>
-    <t>properties.properties.properties.address_city</t>
+    <t>properties.address_city</t>
   </si>
   <si>
     <t>address_county</t>
   </si>
   <si>
-    <t>properties.properties.properties.address_county</t>
+    <t>properties.address_county</t>
   </si>
   <si>
     <t>address_same_as_case</t>
   </si>
   <si>
-    <t>properties.properties.properties.address_same_as_case</t>
+    <t>properties.address_same_as_case</t>
   </si>
   <si>
     <t>address_state</t>
   </si>
   <si>
-    <t>properties.properties.properties.address_state</t>
+    <t>properties.address_state</t>
   </si>
   <si>
     <t>address_street</t>
   </si>
   <si>
-    <t>properties.properties.properties.address_street</t>
+    <t>properties.address_street</t>
   </si>
   <si>
     <t>address_zip</t>
   </si>
   <si>
-    <t>properties.properties.properties.address_zip</t>
+    <t>properties.address_zip</t>
   </si>
   <si>
     <t>age</t>
   </si>
   <si>
-    <t>properties.properties.properties.age</t>
+    <t>properties.age</t>
   </si>
   <si>
     <t>age_range</t>
   </si>
   <si>
-    <t>properties.properties.properties.age_range</t>
+    <t>properties.age_range</t>
   </si>
   <si>
     <t>airline</t>
   </si>
   <si>
-    <t>properties.properties.properties.airline</t>
+    <t>properties.airline</t>
   </si>
   <si>
     <t>arrival_date_to_new_york</t>
   </si>
   <si>
-    <t>properties.properties.properties.arrival_date_to_new_york</t>
+    <t>properties.arrival_date_to_new_york</t>
   </si>
   <si>
     <t>assigned_to_primary_checkin_case_id</t>
   </si>
   <si>
-    <t>properties.properties.properties.assigned_to_primary_checkin_case_id</t>
+    <t>properties.assigned_to_primary_checkin_case_id</t>
   </si>
   <si>
     <t>assigned_to_primary_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.assigned_to_primary_name</t>
+    <t>properties.assigned_to_primary_name</t>
   </si>
   <si>
     <t>assigned_to_primary_username</t>
   </si>
   <si>
-    <t>properties.properties.properties.assigned_to_primary_username</t>
+    <t>properties.assigned_to_primary_username</t>
   </si>
   <si>
     <t>assigned_to_temp_checkin_case_id</t>
   </si>
   <si>
-    <t>properties.properties.properties.assigned_to_temp_checkin_case_id</t>
+    <t>properties.assigned_to_temp_checkin_case_id</t>
   </si>
   <si>
     <t>assigned_to_temp_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.assigned_to_temp_name</t>
+    <t>properties.assigned_to_temp_name</t>
   </si>
   <si>
     <t>assigned_to_temp_username</t>
   </si>
   <si>
-    <t>properties.properties.properties.assigned_to_temp_username</t>
+    <t>properties.assigned_to_temp_username</t>
   </si>
   <si>
     <t>at_home</t>
   </si>
   <si>
-    <t>properties.properties.properties.at_home</t>
+    <t>properties.at_home</t>
   </si>
   <si>
     <t>auto_close_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.auto_close_date</t>
+    <t>properties.auto_close_date</t>
   </si>
   <si>
     <t>bus_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.bus_date</t>
+    <t>properties.bus_date</t>
   </si>
   <si>
     <t>bus_line</t>
   </si>
   <si>
-    <t>properties.properties.properties.bus_line</t>
+    <t>properties.bus_line</t>
   </si>
   <si>
     <t>car_service_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.car_service_date</t>
+    <t>properties.car_service_date</t>
   </si>
   <si>
     <t>car_service_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.car_service_name</t>
+    <t>properties.car_service_name</t>
   </si>
   <si>
     <t>case_link</t>
   </si>
   <si>
-    <t>properties.properties.properties.case_link</t>
+    <t>properties.case_link</t>
   </si>
   <si>
     <t>close_base_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.close_base_date</t>
+    <t>properties.close_base_date</t>
   </si>
   <si>
     <t>closed</t>
   </si>
   <si>
-    <t>properties.properties.properties.closed</t>
-  </si>
-  <si>
     <t>closed_by_username</t>
   </si>
   <si>
-    <t>properties.properties.properties.closed_by_username</t>
+    <t>properties.closed_by_username</t>
   </si>
   <si>
     <t>closed_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.closed_date</t>
+    <t>properties.closed_date</t>
   </si>
   <si>
     <t>commcare_email_address</t>
   </si>
   <si>
-    <t>properties.properties.properties.commcare_email_address</t>
+    <t>properties.commcare_email_address</t>
   </si>
   <si>
     <t>contact_auto_close_exposure_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.contact_auto_close_exposure_date</t>
+    <t>properties.contact_auto_close_exposure_date</t>
   </si>
   <si>
     <t>contact_id</t>
   </si>
   <si>
-    <t>properties.properties.properties.contact_id</t>
+    <t>properties.contact_id</t>
   </si>
   <si>
     <t>contact_notes</t>
   </si>
   <si>
-    <t>properties.properties.properties.contact_notes</t>
+    <t>properties.contact_notes</t>
   </si>
   <si>
     <t>contact_number</t>
   </si>
   <si>
-    <t>properties.properties.properties.contact_number</t>
+    <t>properties.contact_number</t>
   </si>
   <si>
     <t>contact_phone_can_receive_sms</t>
   </si>
   <si>
-    <t>properties.properties.properties.contact_phone_can_receive_sms</t>
+    <t>properties.contact_phone_can_receive_sms</t>
   </si>
   <si>
     <t>contact_phone_number</t>
   </si>
   <si>
-    <t>properties.properties.properties.contact_phone_number</t>
+    <t>properties.contact_phone_number</t>
   </si>
   <si>
     <t>contact_phone_number_is_verified</t>
   </si>
   <si>
-    <t>properties.properties.properties.contact_phone_number_is_verified</t>
+    <t>properties.contact_phone_number_is_verified</t>
   </si>
   <si>
     <t>contact_status</t>
   </si>
   <si>
-    <t>properties.properties.properties.contact_status</t>
+    <t>properties.contact_status</t>
   </si>
   <si>
     <t>contact_type</t>
   </si>
   <si>
-    <t>properties.properties.properties.contact_type</t>
+    <t>properties.contact_type</t>
   </si>
   <si>
     <t>contact_type_other</t>
   </si>
   <si>
-    <t>properties.properties.properties.contact_type_other</t>
+    <t>properties.contact_type_other</t>
   </si>
   <si>
     <t>converted_to_patient</t>
   </si>
   <si>
-    <t>properties.properties.properties.converted_to_patient</t>
+    <t>properties.converted_to_patient</t>
   </si>
   <si>
     <t>converted_to_patient_case_id</t>
   </si>
   <si>
-    <t>properties.properties.properties.converted_to_patient_case_id</t>
+    <t>properties.converted_to_patient_case_id</t>
   </si>
   <si>
     <t>converted_to_pui</t>
   </si>
   <si>
-    <t>properties.properties.properties.converted_to_pui</t>
+    <t>properties.converted_to_pui</t>
   </si>
   <si>
     <t>converted_to_pui_case_id</t>
   </si>
   <si>
-    <t>properties.properties.properties.converted_to_pui_case_id</t>
+    <t>properties.converted_to_pui_case_id</t>
   </si>
   <si>
     <t>county_commcare_domain</t>
   </si>
   <si>
-    <t>properties.properties.properties.county_commcare_domain</t>
+    <t>properties.county_commcare_domain</t>
   </si>
   <si>
     <t>county_display</t>
   </si>
   <si>
-    <t>properties.properties.properties.county_display</t>
+    <t>properties.county_display</t>
   </si>
   <si>
     <t>current_status</t>
   </si>
   <si>
-    <t>properties.properties.properties.current_status</t>
+    <t>properties.current_status</t>
   </si>
   <si>
     <t>date_display</t>
   </si>
   <si>
-    <t>properties.properties.properties.date_display</t>
+    <t>properties.date_display</t>
   </si>
   <si>
     <t>date_of_death</t>
   </si>
   <si>
-    <t>properties.properties.properties.date_of_death</t>
+    <t>properties.date_of_death</t>
   </si>
   <si>
     <t>date_of_last_sms_response</t>
   </si>
   <si>
-    <t>properties.properties.properties.date_of_last_sms_response</t>
+    <t>properties.date_of_last_sms_response</t>
   </si>
   <si>
     <t>days_since_last_sms_response</t>
   </si>
   <si>
-    <t>properties.properties.properties.days_since_last_sms_response</t>
+    <t>properties.days_since_last_sms_response</t>
   </si>
   <si>
     <t>deceased</t>
   </si>
   <si>
-    <t>properties.properties.properties.deceased</t>
+    <t>properties.deceased</t>
   </si>
   <si>
     <t>demo_sms_time</t>
   </si>
   <si>
-    <t>properties.properties.properties.demo_sms_time</t>
+    <t>properties.demo_sms_time</t>
   </si>
   <si>
     <t>dob</t>
   </si>
   <si>
-    <t>properties.properties.properties.dob</t>
+    <t>properties.dob</t>
   </si>
   <si>
     <t>dob_known</t>
   </si>
   <si>
-    <t>properties.properties.properties.dob_known</t>
+    <t>properties.dob_known</t>
   </si>
   <si>
     <t>duplicate_of_case_id</t>
   </si>
   <si>
-    <t>properties.properties.properties.duplicate_of_case_id</t>
+    <t>properties.duplicate_of_case_id</t>
   </si>
   <si>
     <t>edd</t>
   </si>
   <si>
-    <t>properties.properties.properties.edd</t>
+    <t>properties.edd</t>
   </si>
   <si>
     <t>ethnicity</t>
   </si>
   <si>
-    <t>properties.properties.properties.ethnicity</t>
+    <t>properties.ethnicity</t>
   </si>
   <si>
     <t>exposed</t>
   </si>
   <si>
-    <t>properties.properties.properties.exposed</t>
+    <t>properties.exposed</t>
   </si>
   <si>
     <t>exposure_close_proximity</t>
   </si>
   <si>
-    <t>properties.properties.properties.exposure_close_proximity</t>
+    <t>properties.exposure_close_proximity</t>
   </si>
   <si>
     <t>exposure_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.exposure_date</t>
+    <t>properties.exposure_date</t>
   </si>
   <si>
     <t>exposure_date_duplicate</t>
   </si>
   <si>
-    <t>properties.properties.properties.exposure_date_duplicate</t>
+    <t>properties.exposure_date_duplicate</t>
   </si>
   <si>
     <t>exposure_type</t>
   </si>
   <si>
-    <t>properties.properties.properties.exposure_type</t>
+    <t>properties.exposure_type</t>
   </si>
   <si>
     <t>exposure_type_other</t>
   </si>
   <si>
-    <t>properties.properties.properties.exposure_type_other</t>
+    <t>properties.exposure_type_other</t>
   </si>
   <si>
     <t>exposure_type_social_event</t>
   </si>
   <si>
-    <t>properties.properties.properties.exposure_type_social_event</t>
+    <t>properties.exposure_type_social_event</t>
   </si>
   <si>
     <t>exposure_type_travel</t>
   </si>
   <si>
-    <t>properties.properties.properties.exposure_type_travel</t>
+    <t>properties.exposure_type_travel</t>
   </si>
   <si>
     <t>final_disposition</t>
   </si>
   <si>
-    <t>properties.properties.properties.final_disposition</t>
+    <t>properties.final_disposition</t>
   </si>
   <si>
     <t>fips</t>
   </si>
   <si>
-    <t>properties.properties.properties.fips</t>
+    <t>properties.fips</t>
   </si>
   <si>
     <t>first_contact_made</t>
   </si>
   <si>
-    <t>properties.properties.properties.first_contact_made</t>
+    <t>properties.first_contact_made</t>
   </si>
   <si>
     <t>first_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.first_name</t>
+    <t>properties.first_name</t>
   </si>
   <si>
     <t>flight</t>
   </si>
   <si>
-    <t>properties.properties.properties.flight</t>
+    <t>properties.flight</t>
   </si>
   <si>
     <t>flight_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.flight_date</t>
+    <t>properties.flight_date</t>
   </si>
   <si>
     <t>full_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.full_name</t>
+    <t>properties.full_name</t>
   </si>
   <si>
     <t>fup_active</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_active</t>
+    <t>properties.fup_active</t>
   </si>
   <si>
     <t>fup_end_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_end_date</t>
+    <t>properties.fup_end_date</t>
   </si>
   <si>
     <t>fup_extend</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_extend</t>
+    <t>properties.fup_extend</t>
   </si>
   <si>
     <t>fup_last_attempt_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_last_attempt_date</t>
+    <t>properties.fup_last_attempt_date</t>
   </si>
   <si>
     <t>fup_last_attempt_made_by_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_last_attempt_made_by_name</t>
+    <t>properties.fup_last_attempt_made_by_name</t>
   </si>
   <si>
     <t>fup_last_attempt_made_by_username</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_last_attempt_made_by_username</t>
+    <t>properties.fup_last_attempt_made_by_username</t>
   </si>
   <si>
     <t>fup_last_attempt_result</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_last_attempt_result</t>
+    <t>properties.fup_last_attempt_result</t>
   </si>
   <si>
     <t>fup_last_attempt_type</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_last_attempt_type</t>
+    <t>properties.fup_last_attempt_type</t>
   </si>
   <si>
     <t>fup_last_successful_attempt_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_last_successful_attempt_date</t>
+    <t>properties.fup_last_successful_attempt_date</t>
   </si>
   <si>
     <t>fup_last_successful_attempt_made_by_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_last_successful_attempt_made_by_name</t>
+    <t>properties.fup_last_successful_attempt_made_by_name</t>
   </si>
   <si>
     <t>fup_last_successful_attempt_made_by_username</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_last_successful_attempt_made_by_username</t>
+    <t>properties.fup_last_successful_attempt_made_by_username</t>
   </si>
   <si>
     <t>fup_last_successful_attempt_result</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_last_successful_attempt_result</t>
+    <t>properties.fup_last_successful_attempt_result</t>
   </si>
   <si>
     <t>fup_last_successful_attempt_type</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_last_successful_attempt_type</t>
+    <t>properties.fup_last_successful_attempt_type</t>
   </si>
   <si>
     <t>fup_method_preferred</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_method_preferred</t>
+    <t>properties.fup_method_preferred</t>
   </si>
   <si>
     <t>fup_method_preferred_display</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_method_preferred_display</t>
+    <t>properties.fup_method_preferred_display</t>
   </si>
   <si>
     <t>fup_most_recent_note</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_most_recent_note</t>
+    <t>properties.fup_most_recent_note</t>
   </si>
   <si>
     <t>fup_needs_sms_followup</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_needs_sms_followup</t>
+    <t>properties.fup_needs_sms_followup</t>
   </si>
   <si>
     <t>fup_next_call_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_next_call_date</t>
+    <t>properties.fup_next_call_date</t>
   </si>
   <si>
     <t>fup_next_method</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_next_method</t>
+    <t>properties.fup_next_method</t>
   </si>
   <si>
     <t>fup_next_type</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_next_type</t>
+    <t>properties.fup_next_type</t>
   </si>
   <si>
     <t>fup_notes</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_notes</t>
+    <t>properties.fup_notes</t>
   </si>
   <si>
     <t>fup_number_attempts</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_number_attempts</t>
+    <t>properties.fup_number_attempts</t>
   </si>
   <si>
     <t>fup_number_successful_attempts</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_number_successful_attempts</t>
+    <t>properties.fup_number_successful_attempts</t>
   </si>
   <si>
     <t>fup_number_unsuccessful_attempts</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_number_unsuccessful_attempts</t>
+    <t>properties.fup_number_unsuccessful_attempts</t>
   </si>
   <si>
     <t>fup_start_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.fup_start_date</t>
+    <t>properties.fup_start_date</t>
   </si>
   <si>
     <t>gaz</t>
   </si>
   <si>
-    <t>properties.properties.properties.gaz</t>
+    <t>properties.gaz</t>
   </si>
   <si>
     <t>gender</t>
   </si>
   <si>
-    <t>properties.properties.properties.gender</t>
+    <t>properties.gender</t>
   </si>
   <si>
     <t>gps</t>
   </si>
   <si>
-    <t>properties.properties.properties.gps</t>
+    <t>properties.gps</t>
   </si>
   <si>
     <t>has_been_deduped</t>
   </si>
   <si>
-    <t>properties.properties.properties.has_been_deduped</t>
+    <t>properties.has_been_deduped</t>
   </si>
   <si>
     <t>has_index_case</t>
   </si>
   <si>
-    <t>properties.properties.properties.has_index_case</t>
+    <t>properties.has_index_case</t>
   </si>
   <si>
     <t>has_phone_number</t>
   </si>
   <si>
-    <t>properties.properties.properties.has_phone_number</t>
+    <t>properties.has_phone_number</t>
   </si>
   <si>
     <t>hcw</t>
   </si>
   <si>
-    <t>properties.properties.properties.hcw</t>
+    <t>properties.hcw</t>
   </si>
   <si>
     <t>hcw_facility_name_addr</t>
   </si>
   <si>
-    <t>properties.properties.properties.hcw_facility_name_addr</t>
+    <t>properties.hcw_facility_name_addr</t>
   </si>
   <si>
     <t>hcw_facility_reference</t>
   </si>
   <si>
-    <t>properties.properties.properties.hcw_facility_reference</t>
+    <t>properties.hcw_facility_reference</t>
   </si>
   <si>
     <t>hemodialysis</t>
   </si>
   <si>
-    <t>properties.properties.properties.hemodialysis</t>
+    <t>properties.hemodialysis</t>
   </si>
   <si>
     <t>high_risk_confirmed</t>
   </si>
   <si>
-    <t>properties.properties.properties.high_risk_confirmed</t>
+    <t>properties.high_risk_confirmed</t>
   </si>
   <si>
     <t>highest_temp_degrees_f</t>
   </si>
   <si>
-    <t>properties.properties.properties.highest_temp_degrees_f</t>
+    <t>properties.highest_temp_degrees_f</t>
   </si>
   <si>
     <t>hospital_admission_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.hospital_admission_date</t>
+    <t>properties.hospital_admission_date</t>
   </si>
   <si>
     <t>hospital_discharge_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.hospital_discharge_date</t>
+    <t>properties.hospital_discharge_date</t>
   </si>
   <si>
     <t>hospital_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.hospital_name</t>
+    <t>properties.hospital_name</t>
   </si>
   <si>
     <t>hospitalized</t>
   </si>
   <si>
-    <t>properties.properties.properties.hospitalized</t>
+    <t>properties.hospitalized</t>
   </si>
   <si>
     <t>household_residents</t>
   </si>
   <si>
-    <t>properties.properties.properties.household_residents</t>
+    <t>properties.household_residents</t>
   </si>
   <si>
     <t>housing</t>
   </si>
   <si>
-    <t>properties.properties.properties.housing</t>
+    <t>properties.housing</t>
   </si>
   <si>
     <t>housing_other</t>
   </si>
   <si>
-    <t>properties.properties.properties.housing_other</t>
+    <t>properties.housing_other</t>
   </si>
   <si>
     <t>icu</t>
   </si>
   <si>
-    <t>properties.properties.properties.icu</t>
+    <t>properties.icu</t>
   </si>
   <si>
     <t>immune_suppression</t>
   </si>
   <si>
-    <t>properties.properties.properties.immune_suppression</t>
+    <t>properties.immune_suppression</t>
   </si>
   <si>
     <t>indices patient</t>
   </si>
   <si>
-    <t>properties.properties.properties.indices patient</t>
+    <t>properties.indices patient</t>
   </si>
   <si>
     <t>interview_complete</t>
   </si>
   <si>
-    <t>properties.properties.properties.interview_complete</t>
+    <t>properties.interview_complete</t>
   </si>
   <si>
     <t>interview_complete_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.interview_complete_date</t>
+    <t>properties.interview_complete_date</t>
   </si>
   <si>
     <t>interview_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.interview_date</t>
+    <t>properties.interview_date</t>
   </si>
   <si>
     <t>interview_disposition</t>
   </si>
   <si>
-    <t>properties.properties.properties.interview_disposition</t>
+    <t>properties.interview_disposition</t>
   </si>
   <si>
     <t>interview_initiated</t>
   </si>
   <si>
-    <t>properties.properties.properties.interview_initiated</t>
+    <t>properties.interview_initiated</t>
   </si>
   <si>
     <t>interview_status</t>
   </si>
   <si>
-    <t>properties.properties.properties.interview_status</t>
+    <t>properties.interview_status</t>
   </si>
   <si>
     <t>interviewee</t>
   </si>
   <si>
-    <t>properties.properties.properties.interviewee</t>
+    <t>properties.interviewee</t>
   </si>
   <si>
     <t>interviewee_other</t>
   </si>
   <si>
-    <t>properties.properties.properties.interviewee_other</t>
+    <t>properties.interviewee_other</t>
   </si>
   <si>
     <t>interviewee_proxy</t>
   </si>
   <si>
-    <t>properties.properties.properties.interviewee_proxy</t>
+    <t>properties.interviewee_proxy</t>
   </si>
   <si>
     <t>interviewer_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.interviewer_name</t>
+    <t>properties.interviewer_name</t>
   </si>
   <si>
     <t>intubated</t>
   </si>
   <si>
-    <t>properties.properties.properties.intubated</t>
+    <t>properties.intubated</t>
   </si>
   <si>
     <t>investigation</t>
   </si>
   <si>
-    <t>properties.properties.properties.investigation</t>
+    <t>properties.investigation</t>
   </si>
   <si>
     <t>investigation_case_id</t>
   </si>
   <si>
-    <t>properties.properties.properties.investigation_case_id</t>
+    <t>properties.investigation_case_id</t>
   </si>
   <si>
     <t>investigation_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.investigation_name</t>
+    <t>properties.investigation_name</t>
   </si>
   <si>
     <t>iq_notes</t>
   </si>
   <si>
-    <t>properties.properties.properties.iq_notes</t>
+    <t>properties.iq_notes</t>
   </si>
   <si>
     <t>iq_referral</t>
   </si>
   <si>
-    <t>properties.properties.properties.iq_referral</t>
+    <t>properties.iq_referral</t>
   </si>
   <si>
     <t>iq_referral_status</t>
   </si>
   <si>
-    <t>properties.properties.properties.iq_referral_status</t>
+    <t>properties.iq_referral_status</t>
   </si>
   <si>
     <t>is_assigned_primary</t>
   </si>
   <si>
-    <t>properties.properties.properties.is_assigned_primary</t>
+    <t>properties.is_assigned_primary</t>
   </si>
   <si>
     <t>is_assigned_temp</t>
   </si>
   <si>
-    <t>properties.properties.properties.is_assigned_temp</t>
+    <t>properties.is_assigned_temp</t>
   </si>
   <si>
     <t>lang_code</t>
   </si>
   <si>
-    <t>properties.properties.properties.lang_code</t>
+    <t>properties.lang_code</t>
   </si>
   <si>
     <t>language_code</t>
   </si>
   <si>
-    <t>properties.properties.properties.language_code</t>
+    <t>properties.language_code</t>
   </si>
   <si>
     <t>last_modified_by_user_username</t>
   </si>
   <si>
-    <t>properties.properties.properties.last_modified_by_user_username</t>
+    <t>properties.last_modified_by_user_username</t>
   </si>
   <si>
     <t>last_modified_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.last_modified_date</t>
+    <t>properties.last_modified_date</t>
   </si>
   <si>
     <t>last_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.last_name</t>
+    <t>properties.last_name</t>
   </si>
   <si>
     <t>location_details</t>
   </si>
   <si>
-    <t>properties.properties.properties.location_details</t>
+    <t>properties.location_details</t>
   </si>
   <si>
     <t>location_quarantine_isolation</t>
   </si>
   <si>
-    <t>properties.properties.properties.location_quarantine_isolation</t>
+    <t>properties.location_quarantine_isolation</t>
   </si>
   <si>
     <t>low_risk_confirmed</t>
   </si>
   <si>
-    <t>properties.properties.properties.low_risk_confirmed</t>
+    <t>properties.low_risk_confirmed</t>
   </si>
   <si>
     <t>monitoring_end_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.monitoring_end_date</t>
+    <t>properties.monitoring_end_date</t>
   </si>
   <si>
     <t>monitoring_start_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.monitoring_start_date</t>
+    <t>properties.monitoring_start_date</t>
   </si>
   <si>
     <t>most_recent_case_note</t>
   </si>
   <si>
-    <t>properties.properties.properties.most_recent_case_note</t>
+    <t>properties.most_recent_case_note</t>
   </si>
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>properties.properties.properties.name</t>
+    <t>properties.name</t>
   </si>
   <si>
     <t>name_and_id</t>
   </si>
   <si>
-    <t>properties.properties.properties.name_and_id</t>
+    <t>properties.name_and_id</t>
   </si>
   <si>
     <t>next_form</t>
   </si>
   <si>
-    <t>properties.properties.properties.next_form</t>
+    <t>properties.next_form</t>
   </si>
   <si>
     <t>number</t>
   </si>
   <si>
-    <t>properties.properties.properties.number</t>
+    <t>properties.number</t>
   </si>
   <si>
     <t>occupation</t>
   </si>
   <si>
-    <t>properties.properties.properties.occupation</t>
+    <t>properties.occupation</t>
   </si>
   <si>
     <t>occupation_other</t>
   </si>
   <si>
-    <t>properties.properties.properties.occupation_other</t>
+    <t>properties.occupation_other</t>
   </si>
   <si>
     <t>occupation_primary</t>
   </si>
   <si>
-    <t>properties.properties.properties.occupation_primary</t>
+    <t>properties.occupation_primary</t>
   </si>
   <si>
     <t>occupation_primary_other</t>
   </si>
   <si>
-    <t>properties.properties.properties.occupation_primary_other</t>
+    <t>properties.occupation_primary_other</t>
   </si>
   <si>
     <t>occupation_primary_workplace</t>
   </si>
   <si>
-    <t>properties.properties.properties.occupation_primary_workplace</t>
+    <t>properties.occupation_primary_workplace</t>
   </si>
   <si>
     <t>occupation_school</t>
   </si>
   <si>
-    <t>properties.properties.properties.occupation_school</t>
+    <t>properties.occupation_school</t>
   </si>
   <si>
     <t>occupation_school_location</t>
   </si>
   <si>
-    <t>properties.properties.properties.occupation_school_location</t>
+    <t>properties.occupation_school_location</t>
   </si>
   <si>
     <t>occupation_secondary</t>
   </si>
   <si>
-    <t>properties.properties.properties.occupation_secondary</t>
+    <t>properties.occupation_secondary</t>
   </si>
   <si>
     <t>occupation_secondary_other</t>
   </si>
   <si>
-    <t>properties.properties.properties.occupation_secondary_other</t>
+    <t>properties.occupation_secondary_other</t>
   </si>
   <si>
     <t>occupation_secondary_workplace</t>
   </si>
   <si>
-    <t>properties.properties.properties.occupation_secondary_workplace</t>
+    <t>properties.occupation_secondary_workplace</t>
   </si>
   <si>
     <t>ongoing_exposure</t>
   </si>
   <si>
-    <t>properties.properties.properties.ongoing_exposure</t>
+    <t>properties.ongoing_exposure</t>
   </si>
   <si>
     <t>ooj</t>
   </si>
   <si>
-    <t>properties.properties.properties.ooj</t>
+    <t>properties.ooj</t>
   </si>
   <si>
     <t>opened_by_username</t>
   </si>
   <si>
-    <t>properties.properties.properties.opened_by_username</t>
+    <t>properties.opened_by_username</t>
   </si>
   <si>
     <t>opened_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.opened_date</t>
+    <t>properties.opened_date</t>
   </si>
   <si>
     <t>owner_id</t>
   </si>
   <si>
-    <t>properties.properties.properties.owner_id</t>
+    <t>properties.owner_id</t>
   </si>
   <si>
     <t>owner_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.owner_name</t>
+    <t>properties.owner_name</t>
   </si>
   <si>
     <t>phone_call_consent</t>
   </si>
   <si>
-    <t>properties.properties.properties.phone_call_consent</t>
+    <t>properties.phone_call_consent</t>
   </si>
   <si>
     <t>phone_home</t>
   </si>
   <si>
-    <t>properties.properties.properties.phone_home</t>
+    <t>properties.phone_home</t>
   </si>
   <si>
     <t>phone_home_display</t>
   </si>
   <si>
-    <t>properties.properties.properties.phone_home_display</t>
+    <t>properties.phone_home_display</t>
   </si>
   <si>
     <t>phone_work</t>
   </si>
   <si>
-    <t>properties.properties.properties.phone_work</t>
+    <t>properties.phone_work</t>
   </si>
   <si>
     <t>phone_work_display</t>
   </si>
   <si>
-    <t>properties.properties.properties.phone_work_display</t>
+    <t>properties.phone_work_display</t>
   </si>
   <si>
     <t>pregnant</t>
   </si>
   <si>
-    <t>properties.properties.properties.pregnant</t>
+    <t>properties.pregnant</t>
   </si>
   <si>
     <t>presumed_positive</t>
   </si>
   <si>
-    <t>properties.properties.properties.presumed_positive</t>
+    <t>properties.presumed_positive</t>
   </si>
   <si>
     <t>primary_language</t>
   </si>
   <si>
-    <t>properties.properties.properties.primary_language</t>
+    <t>properties.primary_language</t>
   </si>
   <si>
     <t>primary_language_other</t>
   </si>
   <si>
-    <t>properties.properties.properties.primary_language_other</t>
+    <t>properties.primary_language_other</t>
   </si>
   <si>
     <t>private_bathroom</t>
   </si>
   <si>
-    <t>properties.properties.properties.private_bathroom</t>
+    <t>properties.private_bathroom</t>
   </si>
   <si>
     <t>provider_affiliated_facility</t>
   </si>
   <si>
-    <t>properties.properties.properties.provider_affiliated_facility</t>
+    <t>properties.provider_affiliated_facility</t>
   </si>
   <si>
     <t>provider_email_address</t>
   </si>
   <si>
-    <t>properties.properties.properties.provider_email_address</t>
+    <t>properties.provider_email_address</t>
   </si>
   <si>
     <t>provider_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.provider_name</t>
+    <t>properties.provider_name</t>
   </si>
   <si>
     <t>provider_phone_number</t>
   </si>
   <si>
-    <t>properties.properties.properties.provider_phone_number</t>
+    <t>properties.provider_phone_number</t>
   </si>
   <si>
     <t>quarantine_end_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.quarantine_end_date</t>
+    <t>properties.quarantine_end_date</t>
   </si>
   <si>
     <t>quarantine_have_food</t>
   </si>
   <si>
-    <t>properties.properties.properties.quarantine_have_food</t>
+    <t>properties.quarantine_have_food</t>
   </si>
   <si>
     <t>quarantine_have_food_help</t>
   </si>
   <si>
-    <t>properties.properties.properties.quarantine_have_food_help</t>
+    <t>properties.quarantine_have_food_help</t>
   </si>
   <si>
     <t>quarantine_need_help</t>
   </si>
   <si>
-    <t>properties.properties.properties.quarantine_need_help</t>
+    <t>properties.quarantine_need_help</t>
   </si>
   <si>
     <t>quarantine_need_help_details</t>
   </si>
   <si>
-    <t>properties.properties.properties.quarantine_need_help_details</t>
+    <t>properties.quarantine_need_help_details</t>
   </si>
   <si>
     <t>quarantine_notice_sent</t>
   </si>
   <si>
-    <t>properties.properties.properties.quarantine_notice_sent</t>
+    <t>properties.quarantine_notice_sent</t>
   </si>
   <si>
     <t>quarantine_notice_sent_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.quarantine_notice_sent_date</t>
+    <t>properties.quarantine_notice_sent_date</t>
   </si>
   <si>
     <t>quarantine_start_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.quarantine_start_date</t>
+    <t>properties.quarantine_start_date</t>
   </si>
   <si>
     <t>race</t>
   </si>
   <si>
-    <t>properties.properties.properties.race</t>
+    <t>properties.race</t>
   </si>
   <si>
     <t>race_specify</t>
   </si>
   <si>
-    <t>properties.properties.properties.race_specify</t>
+    <t>properties.race_specify</t>
   </si>
   <si>
     <t>registration_user</t>
   </si>
   <si>
-    <t>properties.properties.properties.registration_user</t>
+    <t>properties.registration_user</t>
   </si>
   <si>
     <t>registration_username</t>
   </si>
   <si>
-    <t>properties.properties.properties.registration_username</t>
+    <t>properties.registration_username</t>
   </si>
   <si>
     <t>relation_to_case</t>
   </si>
   <si>
-    <t>properties.properties.properties.relation_to_case</t>
+    <t>properties.relation_to_case</t>
   </si>
   <si>
     <t>relation_to_case_other</t>
   </si>
   <si>
-    <t>properties.properties.properties.relation_to_case_other</t>
+    <t>properties.relation_to_case_other</t>
   </si>
   <si>
     <t>risk</t>
   </si>
   <si>
-    <t>properties.properties.properties.risk</t>
+    <t>properties.risk</t>
   </si>
   <si>
     <t>risk_calculated</t>
   </si>
   <si>
-    <t>properties.properties.properties.risk_calculated</t>
+    <t>properties.risk_calculated</t>
   </si>
   <si>
     <t>risk_override_reason</t>
   </si>
   <si>
-    <t>properties.properties.properties.risk_override_reason</t>
+    <t>properties.risk_override_reason</t>
   </si>
   <si>
     <t>risk_presumed</t>
   </si>
   <si>
-    <t>properties.properties.properties.risk_presumed</t>
+    <t>properties.risk_presumed</t>
   </si>
   <si>
     <t>risk_presumed_detailed</t>
   </si>
   <si>
-    <t>properties.properties.properties.risk_presumed_detailed</t>
+    <t>properties.risk_presumed_detailed</t>
   </si>
   <si>
     <t>risk_presumed_detailed_note</t>
   </si>
   <si>
-    <t>properties.properties.properties.risk_presumed_detailed_note</t>
+    <t>properties.risk_presumed_detailed_note</t>
   </si>
   <si>
     <t>risk_sort</t>
   </si>
   <si>
-    <t>properties.properties.properties.risk_sort</t>
+    <t>properties.risk_sort</t>
   </si>
   <si>
     <t>seat_number</t>
   </si>
   <si>
-    <t>properties.properties.properties.seat_number</t>
+    <t>properties.seat_number</t>
   </si>
   <si>
     <t>self_isolate_end_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.self_isolate_end_date</t>
+    <t>properties.self_isolate_end_date</t>
   </si>
   <si>
     <t>self_isolate_possible</t>
   </si>
   <si>
-    <t>properties.properties.properties.self_isolate_possible</t>
+    <t>properties.self_isolate_possible</t>
   </si>
   <si>
     <t>self_isolate_possible_why_not</t>
   </si>
   <si>
-    <t>properties.properties.properties.self_isolate_possible_why_not</t>
+    <t>properties.self_isolate_possible_why_not</t>
   </si>
   <si>
     <t>self_isolate_start_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.self_isolate_start_date</t>
+    <t>properties.self_isolate_start_date</t>
   </si>
   <si>
     <t>sms_contact_me_request</t>
   </si>
   <si>
-    <t>properties.properties.properties.sms_contact_me_request</t>
+    <t>properties.sms_contact_me_request</t>
   </si>
   <si>
     <t>sms_contact_me_request_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.sms_contact_me_request_date</t>
+    <t>properties.sms_contact_me_request_date</t>
   </si>
   <si>
     <t>sms_contact_me_request_reason</t>
   </si>
   <si>
-    <t>properties.properties.properties.sms_contact_me_request_reason</t>
+    <t>properties.sms_contact_me_request_reason</t>
   </si>
   <si>
     <t>sms_contact_me_trigger</t>
   </si>
   <si>
-    <t>properties.properties.properties.sms_contact_me_trigger</t>
+    <t>properties.sms_contact_me_trigger</t>
   </si>
   <si>
     <t>sms_home_phone</t>
   </si>
   <si>
-    <t>properties.properties.properties.sms_home_phone</t>
+    <t>properties.sms_home_phone</t>
   </si>
   <si>
     <t>sms_primary_language</t>
   </si>
   <si>
-    <t>properties.properties.properties.sms_primary_language</t>
+    <t>properties.sms_primary_language</t>
   </si>
   <si>
     <t>sms_survey_active</t>
   </si>
   <si>
-    <t>properties.properties.properties.sms_survey_active</t>
+    <t>properties.sms_survey_active</t>
   </si>
   <si>
     <t>sms_survey_consent</t>
   </si>
   <si>
-    <t>properties.properties.properties.sms_survey_consent</t>
+    <t>properties.sms_survey_consent</t>
   </si>
   <si>
     <t>sms_survey_end_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.sms_survey_end_date</t>
+    <t>properties.sms_survey_end_date</t>
   </si>
   <si>
     <t>sms_survey_start_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.sms_survey_start_date</t>
+    <t>properties.sms_survey_start_date</t>
   </si>
   <si>
     <t>sms_survey_start_date_default</t>
   </si>
   <si>
-    <t>properties.properties.properties.sms_survey_start_date_default</t>
+    <t>properties.sms_survey_start_date_default</t>
   </si>
   <si>
     <t>sms_survey_time_of_day</t>
   </si>
   <si>
-    <t>properties.properties.properties.sms_survey_time_of_day</t>
+    <t>properties.sms_survey_time_of_day</t>
   </si>
   <si>
     <t>sms_unsubscribe</t>
   </si>
   <si>
-    <t>properties.properties.properties.sms_unsubscribe</t>
+    <t>properties.sms_unsubscribe</t>
   </si>
   <si>
     <t>sms_unsubscribe_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.sms_unsubscribe_date</t>
+    <t>properties.sms_unsubscribe_date</t>
   </si>
   <si>
     <t>source_county_display</t>
   </si>
   <si>
-    <t>properties.properties.properties.source_county_display</t>
+    <t>properties.source_county_display</t>
   </si>
   <si>
     <t>source_county_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.source_county_name</t>
+    <t>properties.source_county_name</t>
   </si>
   <si>
     <t>specify_facility_name_and_address</t>
   </si>
   <si>
-    <t>properties.properties.properties.specify_facility_name_and_address</t>
+    <t>properties.specify_facility_name_and_address</t>
   </si>
   <si>
     <t>state_traveled_from</t>
   </si>
   <si>
-    <t>properties.properties.properties.state_traveled_from</t>
+    <t>properties.state_traveled_from</t>
   </si>
   <si>
     <t>stub</t>
   </si>
   <si>
-    <t>properties.properties.properties.stub</t>
+    <t>properties.stub</t>
   </si>
   <si>
     <t>subway_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.subway_date</t>
+    <t>properties.subway_date</t>
   </si>
   <si>
     <t>subway_information</t>
   </si>
   <si>
-    <t>properties.properties.properties.subway_information</t>
+    <t>properties.subway_information</t>
   </si>
   <si>
     <t>symptom_count</t>
   </si>
   <si>
-    <t>properties.properties.properties.symptom_count</t>
+    <t>properties.symptom_count</t>
   </si>
   <si>
     <t>symptom_onset_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.symptom_onset_date</t>
+    <t>properties.symptom_onset_date</t>
   </si>
   <si>
     <t>symptomatic</t>
   </si>
   <si>
-    <t>properties.properties.properties.symptomatic</t>
+    <t>properties.symptomatic</t>
   </si>
   <si>
     <t>symptomatic_sms</t>
   </si>
   <si>
-    <t>properties.properties.properties.symptomatic_sms</t>
+    <t>properties.symptomatic_sms</t>
   </si>
   <si>
     <t>symptoms_other</t>
   </si>
   <si>
-    <t>properties.properties.properties.symptoms_other</t>
+    <t>properties.symptoms_other</t>
   </si>
   <si>
     <t>symptoms_selected</t>
   </si>
   <si>
-    <t>properties.properties.properties.symptoms_selected</t>
+    <t>properties.symptoms_selected</t>
   </si>
   <si>
     <t>tested_positive</t>
   </si>
   <si>
-    <t>properties.properties.properties.tested_positive</t>
+    <t>properties.tested_positive</t>
   </si>
   <si>
     <t>tested_positive_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.tested_positive_date</t>
+    <t>properties.tested_positive_date</t>
   </si>
   <si>
     <t>train_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.train_date</t>
+    <t>properties.train_date</t>
   </si>
   <si>
     <t>train_information</t>
   </si>
   <si>
-    <t>properties.properties.properties.train_information</t>
+    <t>properties.train_information</t>
   </si>
   <si>
     <t>transfer_date</t>
   </si>
   <si>
-    <t>properties.properties.properties.transfer_date</t>
+    <t>properties.transfer_date</t>
   </si>
   <si>
     <t>transfer_destination_county_domain</t>
   </si>
   <si>
-    <t>properties.properties.properties.transfer_destination_county_domain</t>
+    <t>properties.transfer_destination_county_domain</t>
   </si>
   <si>
     <t>transfer_destination_county_id</t>
   </si>
   <si>
-    <t>properties.properties.properties.transfer_destination_county_id</t>
+    <t>properties.transfer_destination_county_id</t>
   </si>
   <si>
     <t>transfer_destination_county_name</t>
   </si>
   <si>
-    <t>properties.properties.properties.transfer_destination_county_name</t>
+    <t>properties.transfer_destination_county_name</t>
   </si>
   <si>
     <t>transfer_note</t>
   </si>
   <si>
-    <t>properties.properties.properties.transfer_note</t>
+    <t>properties.transfer_note</t>
   </si>
   <si>
     <t>transfer_status</t>
   </si>
   <si>
-    <t>properties.properties.properties.transfer_status</t>
+    <t>properties.transfer_status</t>
   </si>
   <si>
     <t>travel_transportation</t>
   </si>
   <si>
-    <t>properties.properties.properties.travel_transportation</t>
+    <t>properties.travel_transportation</t>
   </si>
   <si>
     <t>underlying_conditions</t>
   </si>
   <si>
-    <t>properties.properties.properties.underlying_conditions</t>
+    <t>properties.underlying_conditions</t>
   </si>
   <si>
     <t>underlying_conditions_other</t>
   </si>
   <si>
-    <t>properties.properties.properties.underlying_conditions_other</t>
+    <t>properties.underlying_conditions_other</t>
   </si>
   <si>
     <t>underlying_conditions_selected</t>
   </si>
   <si>
-    <t>properties.properties.properties.underlying_conditions_selected</t>
+    <t>properties.underlying_conditions_selected</t>
   </si>
 </sst>
 </file>
@@ -1594,15 +1588,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -1895,7 +1889,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G254"/>
+  <dimension ref="A1:G253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1946,215 +1940,215 @@
     </row>
     <row r="3" spans="1:7">
       <c r="E3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="E5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="E6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="E7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="E8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="E9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="E10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="E11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="E12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="E13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="E14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="E15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="E16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="E17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="E18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="E19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="E20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="E21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="E22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="E23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="E24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="E25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="E26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="E27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="E28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="E29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F29" t="s">
         <v>64</v>
@@ -3952,15 +3946,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="254" spans="1:7">
-      <c r="E254" t="s">
-        <v>513</v>
-      </c>
-      <c r="F254" t="s">
-        <v>514</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>